<commit_message>
quick update for better user reading
</commit_message>
<xml_diff>
--- a/pages/trail_list.xlsx
+++ b/pages/trail_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\veron\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mason\Desktop\118iGoldenTeam\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4FEEF4-315D-41C4-8726-B8F15408D54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0275E23A-FF6F-4B77-BAE9-96C6D103548F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="380" windowWidth="19200" windowHeight="9610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,9 +396,6 @@
     <t>1200'</t>
   </si>
   <si>
-    <t>A vigorous uphill trip begins at CA 12 and follows Hood Creek through forests and meadows, past several ponds, and then climbs to the top of 2,730-foot Hood Mountain for distant views. After the f irst mile, the 2017 Nuns Fire burned through most of the trail corridor.</t>
-  </si>
-  <si>
     <t>Jack London State Historic Park and East Slope Sonoma Mountain Trail</t>
   </si>
   <si>
@@ -1011,6 +1008,9 @@
   </si>
   <si>
     <t>longitude</t>
+  </si>
+  <si>
+    <t>A vigorous uphill trip begins at CA 12 and follows Hood Creek through forests and meadows, past several ponds, and then climbs to the top of 2,730-foot Hood Mountain for distant views. After the first mile, the 2017 Nuns Fire burned through most of the trail corridor.</t>
   </si>
 </sst>
 </file>
@@ -1368,16 +1368,16 @@
   </sheetPr>
   <dimension ref="A1:O85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="77.08984375" customWidth="1"/>
-    <col min="8" max="8" width="32.6328125" customWidth="1"/>
-    <col min="11" max="11" width="13.6328125" customWidth="1"/>
-    <col min="12" max="12" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="77.140625" customWidth="1"/>
+    <col min="8" max="8" width="32.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
     <col min="13" max="13" width="22" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1419,7 +1419,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>12</v>
@@ -2685,18 +2685,18 @@
         <v>18</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>122</v>
+        <v>316</v>
       </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B30" s="7">
         <v>3.4</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>16</v>
@@ -2711,7 +2711,7 @@
         <v>18</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I30" s="12" t="s">
         <v>18</v>
@@ -2732,18 +2732,18 @@
         <v>18</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:15">
       <c r="A31" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B31" s="7">
         <v>5.3</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>16</v>
@@ -2765,7 +2765,7 @@
         <v>18</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L31" s="5">
         <v>38.356833100000003</v>
@@ -2777,18 +2777,18 @@
         <v>18</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:15">
       <c r="A32" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B32" s="7">
         <v>5.9</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>28</v>
@@ -2803,7 +2803,7 @@
         <v>18</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I32" s="12" t="s">
         <v>18</v>
@@ -2824,18 +2824,18 @@
         <v>18</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B33" s="7">
         <v>5.2</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>28</v>
@@ -2867,18 +2867,18 @@
         <v>18</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B34" s="7">
         <v>4.0999999999999996</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>33</v>
@@ -2910,18 +2910,18 @@
         <v>18</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:15">
       <c r="A35" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B35" s="7">
         <v>4</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>16</v>
@@ -2943,7 +2943,7 @@
         <v>19</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L35" s="5">
         <v>37.997875100000002</v>
@@ -2955,18 +2955,18 @@
         <v>17</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:15">
       <c r="A36" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B36" s="7">
         <v>3.2</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>28</v>
@@ -3000,18 +3000,18 @@
         <v>18</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:15">
       <c r="A37" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B37" s="7">
         <v>4.3</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>28</v>
@@ -3026,7 +3026,7 @@
         <v>17</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I37" s="12" t="s">
         <v>18</v>
@@ -3047,18 +3047,18 @@
         <v>18</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B38" s="7">
         <v>3.1</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>28</v>
@@ -3092,18 +3092,18 @@
         <v>18</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:15">
       <c r="A39" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B39" s="7">
         <v>5.2</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>28</v>
@@ -3125,7 +3125,7 @@
         <v>17</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L39" s="5">
         <v>37.832689000000002</v>
@@ -3137,18 +3137,18 @@
         <v>18</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:15">
       <c r="A40" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B40" s="7">
         <v>2.2000000000000002</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>33</v>
@@ -3163,7 +3163,7 @@
         <v>17</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I40" s="12" t="s">
         <v>18</v>
@@ -3184,18 +3184,18 @@
         <v>18</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:15">
       <c r="A41" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B41" s="7">
         <v>3.9</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>28</v>
@@ -3211,7 +3211,7 @@
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J41" s="12" t="s">
         <v>17</v>
@@ -3229,18 +3229,18 @@
         <v>18</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:15">
       <c r="A42" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B42" s="7">
         <v>13.5</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>16</v>
@@ -3262,7 +3262,7 @@
         <v>17</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L42" s="5">
         <v>37.5284476</v>
@@ -3274,18 +3274,18 @@
         <v>18</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:15">
       <c r="A43" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B43" s="7">
         <v>4.9000000000000004</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>28</v>
@@ -3300,16 +3300,16 @@
         <v>17</v>
       </c>
       <c r="H43" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="I43" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" s="12" t="s">
         <v>173</v>
-      </c>
-      <c r="I43" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J43" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K43" s="12" t="s">
-        <v>174</v>
       </c>
       <c r="L43" s="5">
         <v>38.510161600000004</v>
@@ -3321,18 +3321,18 @@
         <v>18</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:15">
       <c r="A44" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B44" s="7">
         <v>4.2</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>16</v>
@@ -3347,7 +3347,7 @@
         <v>18</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I44" s="12" t="s">
         <v>18</v>
@@ -3356,7 +3356,7 @@
         <v>17</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L44" s="5">
         <v>38.120198000000002</v>
@@ -3368,12 +3368,12 @@
         <v>18</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:15">
       <c r="A45" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B45" s="7">
         <v>2.9</v>
@@ -3394,7 +3394,7 @@
         <v>18</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>18</v>
@@ -3413,18 +3413,18 @@
         <v>18</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:15">
       <c r="A46" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B46" s="7">
         <v>3.5</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>28</v>
@@ -3448,7 +3448,7 @@
         <v>19</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L46" s="5">
         <v>37.015564900000001</v>
@@ -3460,18 +3460,18 @@
         <v>18</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:15">
       <c r="A47" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B47" s="7">
         <v>6.4</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>28</v>
@@ -3486,16 +3486,16 @@
         <v>17</v>
       </c>
       <c r="H47" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K47" s="12" t="s">
         <v>187</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J47" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>188</v>
       </c>
       <c r="L47" s="5">
         <v>37.903992700000003</v>
@@ -3507,18 +3507,18 @@
         <v>18</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:15">
       <c r="A48" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B48" s="7">
         <v>5.5</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>28</v>
@@ -3540,7 +3540,7 @@
         <v>19</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L48" s="5">
         <v>37.878906800000003</v>
@@ -3552,18 +3552,18 @@
         <v>18</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B49" s="7">
         <v>4.5</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>28</v>
@@ -3585,7 +3585,7 @@
         <v>17</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L49" s="5">
         <v>37.665973200000003</v>
@@ -3597,18 +3597,18 @@
         <v>18</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:15">
       <c r="A50" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B50" s="7">
         <v>6.8</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>33</v>
@@ -3623,7 +3623,7 @@
         <v>17</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I50" s="8" t="s">
         <v>18</v>
@@ -3632,7 +3632,7 @@
         <v>17</v>
       </c>
       <c r="K50" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L50" s="5">
         <v>38.591972200000001</v>
@@ -3644,18 +3644,18 @@
         <v>18</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B51" s="7">
         <v>3.9</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>33</v>
@@ -3677,7 +3677,7 @@
         <v>19</v>
       </c>
       <c r="K51" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L51" s="5">
         <v>37.3696944</v>
@@ -3689,18 +3689,18 @@
         <v>18</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="A52" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B52" s="7">
         <v>6.5</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>16</v>
@@ -3716,7 +3716,7 @@
       </c>
       <c r="H52" s="13"/>
       <c r="I52" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J52" s="8" t="s">
         <v>17</v>
@@ -3734,18 +3734,18 @@
         <v>18</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="53" spans="1:15">
       <c r="A53" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B53" s="7">
         <v>2.7</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>28</v>
@@ -3767,7 +3767,7 @@
         <v>17</v>
       </c>
       <c r="K53" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L53" s="5">
         <v>37.971638900000002</v>
@@ -3779,18 +3779,18 @@
         <v>18</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="54" spans="1:15">
       <c r="A54" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B54" s="7">
         <v>5.8</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>16</v>
@@ -3812,7 +3812,7 @@
         <v>17</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L54" s="5">
         <v>37.428880499999998</v>
@@ -3824,18 +3824,18 @@
         <v>18</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="55" spans="1:15">
       <c r="A55" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B55" s="7">
         <v>7.5</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>28</v>
@@ -3857,7 +3857,7 @@
         <v>17</v>
       </c>
       <c r="K55" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L55" s="5">
         <v>37.831671999999998</v>
@@ -3869,18 +3869,18 @@
         <v>18</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:15">
       <c r="A56" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B56" s="7">
         <v>4.5</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>16</v>
@@ -3895,7 +3895,7 @@
         <v>17</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I56" s="8" t="s">
         <v>18</v>
@@ -3916,18 +3916,18 @@
         <v>18</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B57" s="7">
         <v>6</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>16</v>
@@ -3942,7 +3942,7 @@
         <v>17</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I57" s="12" t="s">
         <v>18</v>
@@ -3961,18 +3961,18 @@
         <v>18</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="58" spans="1:15">
       <c r="A58" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B58" s="7">
         <v>5.5</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>16</v>
@@ -4000,18 +4000,18 @@
         <v>18</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B59" s="7">
         <v>4.2</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>28</v>
@@ -4026,7 +4026,7 @@
         <v>17</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I59" s="8" t="s">
         <v>18</v>
@@ -4047,18 +4047,18 @@
         <v>18</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B60" s="7">
         <v>10.8</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>28</v>
@@ -4092,18 +4092,18 @@
         <v>17</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:15">
       <c r="A61" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B61" s="7">
         <v>9.9</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>28</v>
@@ -4118,10 +4118,10 @@
         <v>17</v>
       </c>
       <c r="H61" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I61" s="14" t="s">
         <v>240</v>
-      </c>
-      <c r="I61" s="14" t="s">
-        <v>241</v>
       </c>
       <c r="J61" s="12" t="s">
         <v>17</v>
@@ -4139,18 +4139,18 @@
         <v>18</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:15">
       <c r="A62" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B62" s="7">
         <v>2.7</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>33</v>
@@ -4182,18 +4182,18 @@
         <v>18</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B63" s="7">
         <v>6</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>16</v>
@@ -4227,18 +4227,18 @@
         <v>17</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="64" spans="1:15">
       <c r="A64" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B64" s="7">
         <v>3.5</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>16</v>
@@ -4272,18 +4272,18 @@
         <v>18</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="65" spans="1:15">
       <c r="A65" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B65" s="7">
         <v>7.1</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>28</v>
@@ -4317,18 +4317,18 @@
         <v>18</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="66" spans="1:15">
       <c r="A66" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B66" s="7">
         <v>7.9</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>28</v>
@@ -4362,18 +4362,18 @@
         <v>18</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="67" spans="1:15">
       <c r="A67" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B67" s="7">
         <v>11.7</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>16</v>
@@ -4395,7 +4395,7 @@
         <v>19</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L67" s="5">
         <v>37.175507813399697</v>
@@ -4407,18 +4407,18 @@
         <v>18</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="68" spans="1:15">
       <c r="A68" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B68" s="7">
         <v>5.3</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>16</v>
@@ -4450,18 +4450,18 @@
         <v>18</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="69" spans="1:15">
       <c r="A69" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B69" s="7">
         <v>4.5999999999999996</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>16</v>
@@ -4495,18 +4495,18 @@
         <v>18</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" spans="1:15">
       <c r="A70" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B70" s="7">
         <v>1.1000000000000001</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>28</v>
@@ -4540,18 +4540,18 @@
         <v>17</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="71" spans="1:15">
       <c r="A71" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B71" s="7">
         <v>3.4</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>28</v>
@@ -4585,18 +4585,18 @@
         <v>18</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="72" spans="1:15">
       <c r="A72" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B72" s="7">
         <v>5</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>28</v>
@@ -4618,7 +4618,7 @@
         <v>19</v>
       </c>
       <c r="K72" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L72" s="5">
         <v>37.312427330197401</v>
@@ -4630,18 +4630,18 @@
         <v>18</v>
       </c>
       <c r="O72" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="73" spans="1:15">
       <c r="A73" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B73" s="7">
         <v>7.6</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>16</v>
@@ -4656,7 +4656,7 @@
         <v>18</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I73" s="8" t="s">
         <v>18</v>
@@ -4675,18 +4675,18 @@
         <v>18</v>
       </c>
       <c r="O73" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="74" spans="1:15">
       <c r="A74" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B74" s="7">
         <v>10.8</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>28</v>
@@ -4708,7 +4708,7 @@
         <v>19</v>
       </c>
       <c r="K74" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L74" s="5">
         <v>38.4176136895708</v>
@@ -4720,18 +4720,18 @@
         <v>18</v>
       </c>
       <c r="O74" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="75" spans="1:15">
       <c r="A75" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B75" s="7">
         <v>3.2</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>28</v>
@@ -4763,18 +4763,18 @@
         <v>18</v>
       </c>
       <c r="O75" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="76" spans="1:15">
       <c r="A76" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B76" s="7">
         <v>6.6</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>28</v>
@@ -4806,18 +4806,18 @@
         <v>18</v>
       </c>
       <c r="O76" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="77" spans="1:15">
       <c r="A77" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B77" s="7">
         <v>2.8</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>16</v>
@@ -4832,7 +4832,7 @@
         <v>17</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I77" s="12" t="s">
         <v>18</v>
@@ -4853,18 +4853,18 @@
         <v>17</v>
       </c>
       <c r="O77" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="78" spans="1:15">
       <c r="A78" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B78" s="7">
         <v>3.2</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>28</v>
@@ -4879,7 +4879,7 @@
         <v>17</v>
       </c>
       <c r="H78" s="12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I78" s="12" t="s">
         <v>18</v>
@@ -4898,18 +4898,18 @@
         <v>18</v>
       </c>
       <c r="O78" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="79" spans="1:15">
       <c r="A79" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B79" s="7">
         <v>9.3000000000000007</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>16</v>
@@ -4925,13 +4925,13 @@
       </c>
       <c r="H79" s="9"/>
       <c r="I79" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J79" s="12" t="s">
         <v>19</v>
       </c>
       <c r="K79" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L79" s="5">
         <v>37.905468168203299</v>
@@ -4943,18 +4943,18 @@
         <v>17</v>
       </c>
       <c r="O79" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="80" spans="1:15">
       <c r="A80" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B80" s="7">
         <v>4.5999999999999996</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>33</v>
@@ -4988,18 +4988,18 @@
         <v>18</v>
       </c>
       <c r="O80" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="81" spans="1:15">
       <c r="A81" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B81" s="7">
         <v>4.8</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>33</v>
@@ -5033,18 +5033,18 @@
         <v>18</v>
       </c>
       <c r="O81" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="82" spans="1:15">
       <c r="A82" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B82" s="7">
         <v>2</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>33</v>
@@ -5078,18 +5078,18 @@
         <v>18</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="83" spans="1:15">
       <c r="A83" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B83" s="7">
         <v>3.3</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>33</v>
@@ -5123,7 +5123,7 @@
         <v>18</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="84" spans="1:15">

</xml_diff>